<commit_message>
20240919 Completado Descargar Excel, Descargar Gráficos en EBA y Metricas
</commit_message>
<xml_diff>
--- a/datos/diccionario_EBA_series_df.xlsx
+++ b/datos/diccionario_EBA_series_df.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruiz\Desktop\Work in Progress\bancos_panel\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Apps\bancos_panel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F678B6D-37F5-4FC2-8235-5851923DFF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF10FADD-AE5B-4F6D-B033-EB06A9535D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12405" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8700" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="listado_nombres_Yahoo" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">listado_nombres_Yahoo!$A$1:$A$22</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -119,9 +132,6 @@
     <t>ROE</t>
   </si>
   <si>
-    <t>Ratio de costos a ingresos</t>
-  </si>
-  <si>
     <t>ROA</t>
   </si>
   <si>
@@ -153,6 +163,9 @@
   </si>
   <si>
     <t>codigo_serie</t>
+  </si>
+  <si>
+    <t>Ratio de eficiencia</t>
   </si>
 </sst>
 </file>
@@ -595,7 +608,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,7 +619,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -689,7 +702,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -697,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -705,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -713,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -721,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -729,7 +742,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -745,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -753,7 +766,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -761,7 +774,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -769,7 +782,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -777,7 +790,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -789,6 +802,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010025A34F53D094394FB21F9DBA6BFE7698" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e7ecd460bafe359a3215e5e4c7378472">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3a2ec7d-e900-4ee0-8b1e-fac67f483317" xmlns:ns3="6cb3014e-c15e-4453-8639-5b8772973515" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be8bf92af2a4fb1c1e1376e9b2342f6b" ns2:_="" ns3:_="">
     <xsd:import namespace="e3a2ec7d-e900-4ee0-8b1e-fac67f483317"/>
@@ -1017,16 +1039,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2D8C0E-0D2C-4690-9BA9-66778D4103C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B631D2E4-1361-44A9-B26B-72C624D3CD94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1043,12 +1064,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2D8C0E-0D2C-4690-9BA9-66778D4103C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>